<commit_message>
Add uv support and dynamic .bundle search
</commit_message>
<xml_diff>
--- a/oils.xlsx
+++ b/oils.xlsx
@@ -703,7 +703,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>25.00</t>
+          <t>15.00</t>
         </is>
       </c>
     </row>
@@ -5128,6 +5128,11 @@
           <t>Penetration Oil</t>
         </is>
       </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="D147" t="n">
         <v>1000</v>
       </c>
@@ -5141,11 +5146,6 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="AE147" t="inlineStr">
-        <is>
-          <t>-0.50</t>
-        </is>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -7056,14 +7056,14 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="J212" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="AA212" t="inlineStr">
-        <is>
-          <t>-0.25</t>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="AC212" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10923,7 +10923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11043,17 +11043,17 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>Reload Speed</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Move Speed</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>Disables Aiming</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Reload Speed</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Move Speed</t>
         </is>
       </c>
     </row>
@@ -11460,7 +11460,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Task Oil</t>
+          <t>Tetris Oil</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -11469,7 +11469,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -11478,19 +11478,19 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-0.25</t>
+          <t>-0.30</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>-0.60</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Tetris Oil</t>
+          <t>Walk Easy Oil</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -11499,7 +11499,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1200</v>
+        <v>250</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -11508,19 +11508,19 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>-0.30</t>
+          <t>-0.15</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>-0.60</t>
+          <t>-0.10</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Walk Easy Oil</t>
+          <t>Whos Counting Oil</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -11529,7 +11529,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -11538,40 +11538,10 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-0.15</t>
+          <t>-0.25</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
-        <is>
-          <t>-0.10</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Whos Counting Oil</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>500</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>-0.25</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
         <is>
           <t>1.00</t>
         </is>
@@ -12357,7 +12327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12386,6 +12356,7 @@
     <col width="10" customWidth="1" min="19" max="19"/>
     <col width="10" customWidth="1" min="20" max="20"/>
     <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12493,6 +12464,11 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>No Organs Drop</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>Jump Power</t>
         </is>
       </c>
@@ -12995,28 +12971,58 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Task Oil</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>900</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>Tech Support Oil</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>1100</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>0.50</t>
         </is>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="V19" t="inlineStr">
         <is>
           <t>-0.70</t>
         </is>
@@ -13194,7 +13200,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>25.00</t>
+          <t>15.00</t>
         </is>
       </c>
     </row>
@@ -17031,7 +17037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17061,7 +17067,6 @@
     <col width="10" customWidth="1" min="20" max="20"/>
     <col width="10" customWidth="1" min="21" max="21"/>
     <col width="10" customWidth="1" min="22" max="22"/>
-    <col width="10" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -17147,35 +17152,30 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Projectile Force Multiplier</t>
+          <t>Bullet Speed</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Bullet Speed</t>
+          <t>No Money Drops</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>No Money Drops</t>
+          <t>Damage%</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Damage%</t>
+          <t>No Organs Drop</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>No Organs Drop</t>
+          <t>Reload Speed</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Reload Speed</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Loot
 Chance
@@ -17489,6 +17489,11 @@
           <t>Penetration Oil</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="D12" t="n">
         <v>1000</v>
       </c>
@@ -17502,11 +17507,6 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>-0.50</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -17557,7 +17557,7 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>-0.50</t>
         </is>
@@ -17587,7 +17587,7 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -17617,7 +17617,7 @@
           <t>3.00</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>-0.30</t>
         </is>
@@ -17647,7 +17647,7 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -17677,7 +17677,7 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="V18" t="inlineStr">
+      <c r="U18" t="inlineStr">
         <is>
           <t>-0.25</t>
         </is>
@@ -17707,7 +17707,7 @@
           <t>1.00</t>
         </is>
       </c>
-      <c r="W19" t="inlineStr">
+      <c r="V19" t="inlineStr">
         <is>
           <t>-0.50</t>
         </is>

</xml_diff>